<commit_message>
add prompt in record sheet
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,10 +504,15 @@
           <t>tasks</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>specific_prompt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -526,7 +531,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>shyam_ghosh@technologymindz.com</t>
+          <t>charlie.brown@example.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -567,13 +572,13 @@
       <c r="M2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-[2025-09-23 18:54:54] The user wants to schedule a meeting and provides a preferred date and time, but there is a misunderstanding about the date.</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-09-23 18:54:54] 1. Schedule a meeting, 2. Send meeting invitation to email</t>
+[2025-09-24 17:43:24] The customer is from the UK, likes football, and has dust allergies, but the conversation didn't go further as the customer didn't express any specific requirements or interests beyond that.</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>he is getting alergies of dust particals</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
db init issue fix
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -512,11 +512,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -551,17 +551,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Healthcare</t>
+          <t>Real Estate</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>D Company</t>
+          <t>C Company</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Texas, USA</t>
+          <t>Berlin, Germany</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -572,7 +572,7 @@
       <c r="M2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-[2025-09-24 17:43:24] The customer is from the UK, likes football, and has dust allergies, but the conversation didn't go further as the customer didn't express any specific requirements or interests beyond that.</t>
+[2025-09-24 22:41:26] The customer confirms it's a good time to talk and inquires about the AI's knowledge of them. The AI recalls the customer's name, association with C company in the real estate industry in Berlin, Germany, and their dust allergy concerns.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>

</xml_diff>

<commit_message>
past date invite fix
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -512,7 +512,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -572,20 +572,20 @@
       <c r="M2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-[2025-09-25 15:57:43] No Notes available.</t>
+[2025-09-25 18:56:26] No Notes available.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-[2025-09-25 15:57:43] No tasks found for this call.</t>
+[2025-09-25 18:56:26] No tasks found for this call.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -645,15 +645,10 @@
       <c r="M3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-[2025-09-25 15:58:42] The user is dealing with dust allergies and wants to schedule a meeting.</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-09-25 15:58:42] 1. Schedule a meeting</t>
-        </is>
-      </c>
+[2025-09-25 18:58:24] The user is dealing with dust allergies and wants to schedule a meeting, but the preferred time provided is outside business hours.</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
           <t>he is getting alergies of dust particals</t>

</xml_diff>

<commit_message>
remove notes from the llm prompt
</commit_message>
<xml_diff>
--- a/resultant_excel.xlsx
+++ b/resultant_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,36 +512,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alice1 Johnson</t>
+          <t>shyam ghosh</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3425142353545</t>
+          <t>8107061392</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>alice.johnson@example.com</t>
+          <t>shyam_ghosh@technologymindz.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Alice is interested in the premium package that includes advanced analytics, priority support, and additional storage capacity. She wants a detailed demo before making the decision.</t>
+          <t>shyam is interested in the premium package that includes advanced analytics, priority support, and additionAal storage capacity. She wants a detailed demo before making the decision.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>initialize-failed</t>
+          <t>completed</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>A Company</t>
+          <t>D Company</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -566,90 +566,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-09-29 19:09:06] No Notes available.</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-09-29 19:09:06] No tasks found for this call.</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>177</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>shyam ghosh</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>8107061392</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>shyam_ghosh@technologymindz.com</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>shyam is interested in the premium package that includes advanced analytics, priority support, and additionAal storage capacity. She wants a detailed demo before making the decision.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Healthcare</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>D Company</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Texas, USA</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-[2025-09-29 19:09:57] AI assistant contacted user Raja regarding premium package interest and attempted to schedule follow-up</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
         <is>
           <t>before  greeting the user, use ai chatbot inquery</t>
         </is>

</xml_diff>